<commit_message>
Major update to version 1.9.9 (see NEWS for details).
git-svn-id: file:///home/git/hedgehog.fhcrc.org/bioconductor/trunk/madman/Rpacks/TPP@109277 bc3139a8-67e5-0310-9ffc-ced21a209358
</commit_message>
<xml_diff>
--- a/inst/example_data/CCR_example_data/Panobinostat_TPP-CCR_config.xlsx
+++ b/inst/example_data/CCR_example_data/Panobinostat_TPP-CCR_config.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>Experiment</t>
   </si>
@@ -56,6 +56,9 @@
   </si>
   <si>
     <t>Panobinostat_1</t>
+  </si>
+  <si>
+    <t>Panobinostat_2</t>
   </si>
 </sst>
 </file>
@@ -458,10 +461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -547,6 +550,44 @@
         <v>12</v>
       </c>
     </row>
+    <row r="3" spans="1:12" ht="15.75">
+      <c r="A3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="2">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0.625</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0.15625</v>
+      </c>
+      <c r="F3" s="1">
+        <v>3.9059999999999997E-2</v>
+      </c>
+      <c r="G3" s="2">
+        <v>9.7699999999999905E-3</v>
+      </c>
+      <c r="H3" s="1">
+        <v>2.4399999999999999E-3</v>
+      </c>
+      <c r="I3" s="1">
+        <v>6.0999999999999997E-4</v>
+      </c>
+      <c r="J3" s="2">
+        <v>1.4999999999999999E-4</v>
+      </c>
+      <c r="K3" s="2">
+        <v>0</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>

</xml_diff>